<commit_message>
update: network get parallel
</commit_message>
<xml_diff>
--- a/7-2.network get parallel/resource/kr2cn.xlsx
+++ b/7-2.network get parallel/resource/kr2cn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AeroCode\Desktop\MyProject\node-napi-benchmark\7-2.network get parallel\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C58F15D-6EB6-4490-A6EE-D8E3D19180AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57BFA27-CE92-46F6-8634-A48E43B6E87C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{495E4641-9371-49E1-9625-91E4161970A5}"/>
+    <workbookView xWindow="8820" yWindow="3810" windowWidth="7500" windowHeight="6000" xr2:uid="{495E4641-9371-49E1-9625-91E4161970A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>youku</t>
+    <t>sogou</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -277,7 +277,7 @@
                     <c:v>baidu</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>youku</c:v>
+                    <c:v>sogou</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -302,16 +302,16 @@
                   <c:v>836</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9816</c:v>
+                  <c:v>1567</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4672</c:v>
+                  <c:v>6508</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3904</c:v>
+                  <c:v>5873</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>761</c:v>
+                  <c:v>1854</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -550,7 +550,7 @@
                     <c:v>baidu</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>youku</c:v>
+                    <c:v>sogou</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -575,16 +575,16 @@
                   <c:v>836</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9816</c:v>
+                  <c:v>1567</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4672</c:v>
+                  <c:v>6508</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3904</c:v>
+                  <c:v>5873</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>761</c:v>
+                  <c:v>1854</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,7 +1240,7 @@
   <dimension ref="B1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1271,7 +1271,7 @@
         <v>916</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="0">SUM(D3:D3)</f>
+        <f t="shared" ref="E3:E10" si="0">SUM(D3:D3)</f>
         <v>916</v>
       </c>
     </row>
@@ -1320,11 +1320,11 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>9816</v>
+        <v>1567</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>9816</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -1332,11 +1332,11 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>4672</v>
+        <v>6508</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>4672</v>
+        <v>6508</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -1344,11 +1344,11 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <v>3904</v>
+        <v>5873</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>3904</v>
+        <v>5873</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -1356,11 +1356,11 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>761</v>
+        <v>1854</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>761</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -1384,6 +1384,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101002000BFFA108DB047B3EFC5DDF5207AF1" ma:contentTypeVersion="2" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="360e30c3308fc58e22752f98ab7121e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0f80c752-7000-4b24-82e0-cc1a08bf636a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0602d9b23f70dd89cb9d3785157d2296" ns3:_="">
     <xsd:import namespace="0f80c752-7000-4b24-82e0-cc1a08bf636a"/>
@@ -1515,15 +1524,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ECB2419-4549-41F4-A2F0-D5D48E12DC82}">
   <ds:schemaRefs>
@@ -1541,6 +1541,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FCEE90F-47AC-44EC-AE83-3091D9608E0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EB26047-8973-49C2-879F-B7DE90AED6CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1556,12 +1564,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FCEE90F-47AC-44EC-AE83-3091D9608E0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>